<commit_message>
Fixed prices and references
</commit_message>
<xml_diff>
--- a/SPARC Capstone Preliminary BOM.xlsx
+++ b/SPARC Capstone Preliminary BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dr_mo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BE1AB3-1C9F-4D93-A1DE-D0C01D3720E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F544D81F-CE8E-48F2-9566-433C5D0F5B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="2490" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
   <si>
     <t>Reference</t>
   </si>
@@ -77,9 +77,6 @@
     <t>445-13048-1-ND</t>
   </si>
   <si>
-    <t>C8</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t>Murata</t>
   </si>
   <si>
-    <t>C7, C9</t>
-  </si>
-  <si>
     <t>490-14002-1-ND</t>
   </si>
   <si>
@@ -135,9 +129,6 @@
   </si>
   <si>
     <t>2057-PH1-03-UA-ND</t>
-  </si>
-  <si>
-    <t>R1-R31</t>
   </si>
   <si>
     <r>
@@ -178,18 +169,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>May need to buy direct from Microchip as Digikey is short of stock</t>
-  </si>
-  <si>
-    <t>U1 Alt</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Microchipdirect.com listing. Cheaper even when factoring shipping</t>
-  </si>
-  <si>
     <t>As specified in given schematic</t>
   </si>
   <si>
@@ -272,6 +251,18 @@
   </si>
   <si>
     <t>Jumper</t>
+  </si>
+  <si>
+    <t>C7, C9, C11, C12</t>
+  </si>
+  <si>
+    <t>C8, C10</t>
+  </si>
+  <si>
+    <t>R1-R62</t>
+  </si>
+  <si>
+    <t>$42.39 From Digikey</t>
   </si>
 </sst>
 </file>
@@ -662,7 +653,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -707,6 +698,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="8" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -990,19 +982,20 @@
   <dimension ref="B1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="61.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1021,7 +1014,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="38" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G2" s="21" t="s">
         <v>10</v>
@@ -1036,7 +1029,7 @@
         <v>6</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
@@ -1053,7 +1046,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G3" s="37" t="s">
         <v>12</v>
@@ -1072,22 +1065,22 @@
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="33" t="s">
         <v>16</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="33" t="s">
-        <v>18</v>
       </c>
       <c r="H4" s="1">
         <v>4</v>
@@ -1103,22 +1096,22 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="33" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="G5" s="33" t="s">
-        <v>23</v>
       </c>
       <c r="H5" s="1">
         <v>2</v>
@@ -1134,22 +1127,22 @@
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="33" t="s">
         <v>24</v>
-      </c>
-      <c r="E6" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="G6" s="33" t="s">
-        <v>26</v>
       </c>
       <c r="H6" s="1">
         <v>1</v>
@@ -1162,27 +1155,27 @@
         <v>0.63</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E7" s="32">
         <v>732511150</v>
       </c>
       <c r="F7" s="34" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H7" s="1">
         <v>2</v>
@@ -1195,27 +1188,27 @@
         <v>12.56</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G8" s="33" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H8" s="1">
         <v>2</v>
@@ -1228,27 +1221,27 @@
         <v>0.38</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="33" t="s">
         <v>30</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="G9" s="33" t="s">
-        <v>32</v>
       </c>
       <c r="H9" s="1">
         <v>1</v>
@@ -1261,27 +1254,27 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="F10" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="33" t="s">
         <v>34</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="G10" s="33" t="s">
-        <v>37</v>
       </c>
       <c r="H10" s="1">
         <v>62</v>
@@ -1297,22 +1290,22 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F11" s="34" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H11" s="24">
         <v>1</v>
@@ -1328,69 +1321,48 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="33" t="s">
         <v>38</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="G12" s="33" t="s">
-        <v>41</v>
       </c>
       <c r="H12" s="1">
         <v>2</v>
       </c>
-      <c r="I12" s="3">
-        <v>42.39</v>
+      <c r="I12" s="42">
+        <v>40.270000000000003</v>
       </c>
       <c r="J12" s="2">
         <f>I12*H12</f>
-        <v>84.78</v>
+        <v>80.540000000000006</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="40" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="19">
-        <v>2</v>
-      </c>
-      <c r="I13" s="15">
-        <v>26.07</v>
-      </c>
-      <c r="J13" s="16">
-        <f>I13*H13</f>
-        <v>52.14</v>
-      </c>
-      <c r="K13" s="17" t="s">
-        <v>46</v>
-      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="17"/>
     </row>
     <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="13"/>
@@ -1401,11 +1373,11 @@
       <c r="G14" s="14"/>
       <c r="H14" s="22"/>
       <c r="I14" s="21" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J14" s="20">
         <f>SUM(J3:J12)</f>
-        <v>121.852</v>
+        <v>117.61199999999999</v>
       </c>
       <c r="K14" s="12"/>
     </row>

</xml_diff>